<commit_message>
UPDATE : Perbaiakn pada select dihalaman index agar menyimpan value select sebelumnya
</commit_message>
<xml_diff>
--- a/uploads/jadwal-dosen.xlsx
+++ b/uploads/jadwal-dosen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF GAMING\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B267D3D-4960-48A1-9971-ECB5C69AC503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11C53A2-EE48-42DD-B0BD-BC49D5260DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3982EF8-5654-4D17-B35A-D4535971505A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="46">
   <si>
     <t>Dr. Eng, DEFRY HAMDHANA, ST.,M.Kom</t>
   </si>
@@ -54,9 +54,6 @@
     <t>WAHYU FUADI, ST, M.IT</t>
   </si>
   <si>
-    <t>EVA DARNILA, ST.,MT, NUNSINA, ST., M.Kom</t>
-  </si>
-  <si>
     <t>EVA DARNILA, ST.,MT</t>
   </si>
   <si>
@@ -75,17 +72,37 @@
     <t>08:30-11:00</t>
   </si>
   <si>
-    <t>Dr., NURDIN, S.KOM, M.KOM,
-HAFIZH AL KAUTSAR AIDILOF, ST.,M.Kom</t>
-  </si>
-  <si>
-    <t>NUNSINA, ST., M.Kom, EVA DARNILA, ST.,MT</t>
-  </si>
-  <si>
-    <t>HAFIZH AL KAUTSAR AIDILOF, ST.,M.Kom, Dr., NURDIN, S.KOM, M.KOM</t>
-  </si>
-  <si>
-    <t>T.Sukma Achriadi Sukiman, S.Kom., M.Kom, ANNI ZULFIA, S.Pd., M.Kom</t>
+    <t>08:00-09:40</t>
+  </si>
+  <si>
+    <t>09:50-11:30</t>
+  </si>
+  <si>
+    <t>11:40-13:20</t>
+  </si>
+  <si>
+    <t>09:40-11:20</t>
+  </si>
+  <si>
+    <t>SUJACKA RETNO, S.T., M.Kom</t>
+  </si>
+  <si>
+    <t>14:30-17:00</t>
+  </si>
+  <si>
+    <t>RINI MEIYANTI, ST.,M.Kom</t>
+  </si>
+  <si>
+    <t>FADLISYAH, S.Si.,MT</t>
+  </si>
+  <si>
+    <t>RIZAL, S.Si, M.IT</t>
+  </si>
+  <si>
+    <t>10:30-13:10</t>
+  </si>
+  <si>
+    <t>AR RAZI, ST.,M.Cs</t>
   </si>
   <si>
     <t>DOSEN</t>
@@ -104,6 +121,57 @@
   </si>
   <si>
     <t>JUMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NUNSINA, ST., M.Kom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NURDIN, S.KOM, M.KOM</t>
+  </si>
+  <si>
+    <t>Dr., NURDIN, S.KOM, M.KOM</t>
+  </si>
+  <si>
+    <t>HAFIZH AL KAUTSAR AIDILOF, ST.,M.Kom</t>
+  </si>
+  <si>
+    <t>T.Sukma Achriadi Sukiman, S.Kom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ANNI ZULFIA, S.Pd., M.Kom</t>
+  </si>
+  <si>
+    <t>CUT AGUSNIAR, S.T., M.Cs</t>
+  </si>
+  <si>
+    <t>LIDYA ROSNITA, S.T., M. Kom</t>
+  </si>
+  <si>
+    <t>RISAWANDI, ST.,M.Kom</t>
+  </si>
+  <si>
+    <t>KOORDINATOR</t>
+  </si>
+  <si>
+    <t>MARYANA, S.Si., M.Si</t>
+  </si>
+  <si>
+    <t>BUSTAMI, S.Si,M.Si</t>
+  </si>
+  <si>
+    <t>Dr, FAJRIANA, S. Si., M.Si</t>
+  </si>
+  <si>
+    <t>11:20-13:00</t>
+  </si>
+  <si>
+    <t>13:30-15:10</t>
+  </si>
+  <si>
+    <t>M.Kom, ANNI ZULFIA, S.Pd., M.Kom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CUT AGUSNIAR, S.T., M.Cs</t>
   </si>
 </sst>
 </file>
@@ -154,10 +222,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D213A8B6-5EDA-4FF4-AC64-4EB77E26D40E}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,22 +566,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -596,12 +670,14 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -610,7 +686,9 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
@@ -620,7 +698,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -632,7 +710,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -644,7 +722,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -656,7 +734,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -668,7 +746,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -692,46 +770,56 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
+      <c r="A20" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
       </c>
@@ -739,68 +827,74 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
+      <c r="A21" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
+      <c r="A22" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D23" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
@@ -810,6 +904,642 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F79" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FIXED & UPDATE : Perbaiki select pada halaman agar menyimpan value yang sudah dipilih agar tidak membuat ulang dan perbarui waktu mulai dan selesai sempro dan sidang
</commit_message>
<xml_diff>
--- a/uploads/jadwal-dosen.xlsx
+++ b/uploads/jadwal-dosen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS TUF GAMING\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B267D3D-4960-48A1-9971-ECB5C69AC503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11C53A2-EE48-42DD-B0BD-BC49D5260DB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3982EF8-5654-4D17-B35A-D4535971505A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="46">
   <si>
     <t>Dr. Eng, DEFRY HAMDHANA, ST.,M.Kom</t>
   </si>
@@ -54,9 +54,6 @@
     <t>WAHYU FUADI, ST, M.IT</t>
   </si>
   <si>
-    <t>EVA DARNILA, ST.,MT, NUNSINA, ST., M.Kom</t>
-  </si>
-  <si>
     <t>EVA DARNILA, ST.,MT</t>
   </si>
   <si>
@@ -75,17 +72,37 @@
     <t>08:30-11:00</t>
   </si>
   <si>
-    <t>Dr., NURDIN, S.KOM, M.KOM,
-HAFIZH AL KAUTSAR AIDILOF, ST.,M.Kom</t>
-  </si>
-  <si>
-    <t>NUNSINA, ST., M.Kom, EVA DARNILA, ST.,MT</t>
-  </si>
-  <si>
-    <t>HAFIZH AL KAUTSAR AIDILOF, ST.,M.Kom, Dr., NURDIN, S.KOM, M.KOM</t>
-  </si>
-  <si>
-    <t>T.Sukma Achriadi Sukiman, S.Kom., M.Kom, ANNI ZULFIA, S.Pd., M.Kom</t>
+    <t>08:00-09:40</t>
+  </si>
+  <si>
+    <t>09:50-11:30</t>
+  </si>
+  <si>
+    <t>11:40-13:20</t>
+  </si>
+  <si>
+    <t>09:40-11:20</t>
+  </si>
+  <si>
+    <t>SUJACKA RETNO, S.T., M.Kom</t>
+  </si>
+  <si>
+    <t>14:30-17:00</t>
+  </si>
+  <si>
+    <t>RINI MEIYANTI, ST.,M.Kom</t>
+  </si>
+  <si>
+    <t>FADLISYAH, S.Si.,MT</t>
+  </si>
+  <si>
+    <t>RIZAL, S.Si, M.IT</t>
+  </si>
+  <si>
+    <t>10:30-13:10</t>
+  </si>
+  <si>
+    <t>AR RAZI, ST.,M.Cs</t>
   </si>
   <si>
     <t>DOSEN</t>
@@ -104,6 +121,57 @@
   </si>
   <si>
     <t>JUMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NUNSINA, ST., M.Kom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> NURDIN, S.KOM, M.KOM</t>
+  </si>
+  <si>
+    <t>Dr., NURDIN, S.KOM, M.KOM</t>
+  </si>
+  <si>
+    <t>HAFIZH AL KAUTSAR AIDILOF, ST.,M.Kom</t>
+  </si>
+  <si>
+    <t>T.Sukma Achriadi Sukiman, S.Kom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ANNI ZULFIA, S.Pd., M.Kom</t>
+  </si>
+  <si>
+    <t>CUT AGUSNIAR, S.T., M.Cs</t>
+  </si>
+  <si>
+    <t>LIDYA ROSNITA, S.T., M. Kom</t>
+  </si>
+  <si>
+    <t>RISAWANDI, ST.,M.Kom</t>
+  </si>
+  <si>
+    <t>KOORDINATOR</t>
+  </si>
+  <si>
+    <t>MARYANA, S.Si., M.Si</t>
+  </si>
+  <si>
+    <t>BUSTAMI, S.Si,M.Si</t>
+  </si>
+  <si>
+    <t>Dr, FAJRIANA, S. Si., M.Si</t>
+  </si>
+  <si>
+    <t>11:20-13:00</t>
+  </si>
+  <si>
+    <t>13:30-15:10</t>
+  </si>
+  <si>
+    <t>M.Kom, ANNI ZULFIA, S.Pd., M.Kom</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CUT AGUSNIAR, S.T., M.Cs</t>
   </si>
 </sst>
 </file>
@@ -154,10 +222,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -473,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D213A8B6-5EDA-4FF4-AC64-4EB77E26D40E}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -492,22 +566,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -596,12 +670,14 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -610,7 +686,9 @@
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="C10" s="1" t="s">
         <v>1</v>
       </c>
@@ -620,7 +698,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
@@ -632,7 +710,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -644,7 +722,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -656,7 +734,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -668,7 +746,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>3</v>
@@ -692,46 +770,56 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
       <c r="D17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>10</v>
+      <c r="A20" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="D20" s="1" t="s">
         <v>1</v>
       </c>
@@ -739,68 +827,74 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>13</v>
+      <c r="A21" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>13</v>
+      <c r="A22" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>1</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D23" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
-      <c r="D24" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
+      <c r="F24" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B25" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
@@ -810,6 +904,642 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D59" s="3"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F65" s="3"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+      <c r="E67" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B77" s="3"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B78" s="3"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+      <c r="E79" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F79" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>